<commit_message>
Update excel export; update package and yarn
</commit_message>
<xml_diff>
--- a/trialverse/excelExportExample.xlsx
+++ b/trialverse/excelExportExample.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Study data" sheetId="1" state="visible" r:id="rId2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="101">
   <si>
     <t xml:space="preserve">Study Information</t>
   </si>
@@ -72,94 +72,76 @@
     <t xml:space="preserve">description</t>
   </si>
   <si>
-    <t xml:space="preserve">treatment</t>
+    <t xml:space="preserve">variable type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">measurement type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">measurement moment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">standard deviation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mean</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N</t>
+  </si>
+  <si>
+    <t xml:space="preserve">count</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fava et al., 1998</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://addis-test.drugis.org/#/users/4/datasets/215004da-4ef3-4979-afb1-24be42bb0ecf/versions/62411d0c-d327-431d-854a-3715b895413a/studies/5e759104-6992-429c-91a4-ff9779c1f14a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A double-blind study of paroxetine, fluoxetine, and placebo in outpatients with major depression</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Randomized</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Double blind</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Completed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Comparison of the efficacy and tolerability of paroxetine and fluoxetine in outpatients with major depression.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Severe depression</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inclusion criteria: The patients were recruited from general and psychiatric practices and clinics. Patients (aged between 18 and 70 years) fulfilling DSM-IV criteria for major depressive episode and with a total score of &gt;= 18 on the first 17 items the HAM-D scale at baseline were eligible for inclusion in the study. A severely depressed patient was defined as having an HAM-D score at baseline of &gt;= 25. Exclusion criteria: A current diagnosis of eating disorders, postpartum depression or anxiety disorders (DSM-IV), or a current or previous diagnosis of any other DSM-IV Axis I or Axis II diagnosis including bipolar disorder or schizophrenia were criteria for exclusion. Patients were also excluded if they had epilepsy or a history of seizure disorder or anticonvulsant treatment; were pregnant, lactating, or of childbearing potential and not taking adequate contraceptive measures; were a suicide risk; were suffering from alcohol/substance abuse, a chronic and unstable physical disease, or one that could explain the symptoms of depression, or clinically meaningful abnormal findings on physical examination. Other reasons for exclusion included an episode duration of less than 2 weeks, a current depressive episode of more than 12 months, a lack of response to at least 2 adequate antidepressant therapies during the current episode, and more than 2 previous episodes that did not respond to adequate antidepressant therapy. Patients who had shown previous hypersensitivity to mirtazapine or sertraline or who had developed serotonergic syndrome on treatment with an SSRI were not permitted to enter the study. The following treatments had to be stopped within the indicated intervals before the start of active study medication: electroconvulsive therapy (3 months), depot neuroleptics (2 months), fluspirilene (1 month), fluoxetine (1 month), monoamine oxidase inhibitors (3 weeks), testosterone and its derivatives (1 week for oral formulations and 3 weeks for intramuscular), benzodiazepines (1 week), St John’s Wort (1 week), sertraline and mirtazapine (current episode), and other psychotropic drugs (1 week). Any formal psychotherapy must have been stopped at least 1 month prior to baseline. Patients were excluded if they used sildenafil or other similar agents.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fluoxetine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">baselineCharacteristic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">continuous</t>
+  </si>
+  <si>
+    <t xml:space="preserve">endpoint</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dichotomous</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fluoxetine + background metformin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Overall population</t>
   </si>
   <si>
     <t xml:space="preserve">id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">variable type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">measurement type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">measurement moment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">standard deviation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mean</t>
-  </si>
-  <si>
-    <t xml:space="preserve">N</t>
-  </si>
-  <si>
-    <t xml:space="preserve">count</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fava et al., 1998</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://addis.drugis.org/#/users/3/datasets/65f9e23d-6e8d-4ccd-aacd-95b672520ce2/studies/01c306bc-a3f4-480c-9c59-c3005d652999</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A double-blind study of paroxetine, fluoxetine, and placebo in outpatients with major depression</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Randomized</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Double blind</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Completed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Comparison of the efficacy and tolerability of paroxetine and fluoxetine in outpatients with major depression.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Severe depression</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Inclusion criteria:
-Outpatients with moderate to moderately severe major depression without a history of mania or hypomania were recruited between 1993 and 1994. For each subject, a Raskin Depression Scale score of at least 8, and larger in value than the Covi Anxiety Scale score was required, as well as a Hamilton Rating Scale for Depression (HAM-D) score of 18 or greater on the first 17 items.
-Exclusion criteria:
-Excluded were patients with the following primary psychiatric diagnoses: schizophrenia, adjustment disorder, bipolar disorder, panic disorder, social phobia, obsessive-compulsive disorder, psychotic depression, and atypical depression. Other exclusions included patients whose HAM-D total score fell by 25% or more between the screen and baseline evaluations, patients with serious concomitant medical illness or significant abnormal laboratory values at screening or baseline, patients with history of seizure disorders (except febrile seizures in childhood), patients judged to have a high suicidal risk by the investigator, patients with a recent history (within 6 months) of alcohol or drug abuse, patients who required therapy with other psychotropic drug within 14 days of baseline (with the exception of chloral hydrate for sleep), patients who received electroconvulsive therapy within 3 months of baseline, were hypersensitive to fluoxetine during a prior treatment period, or used any investigational drug within 30 days of baseline, and patients previously treated with paroxetine. Women of childbearing age were excluded if they had positive pregnancy tests or did not practice medically accepted means of birth control. Screening included pregnancy testing for women, body weight determination, medical history, physical examination, 12-lead ECG, vital signs (including screen for postural hypotension), laboratory testing, including: hematology (hematocrit, hemoglobin, WBC with differential, platelet count); blood chemistry (alkaline phosphatase, BUN, creatinine, AST, ALT, total bilirubin, total T3, and total T4); and urinalysis (if dipstick was positive for blood or protein, full microscopy was performed). Psychiatric screening included: DSM-III-R multi-axial diagnostic evaluations, 21-item HAM-D, Raskin Depression Scale, Covi Anxiety Scale, and a detailed psychiatric history.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fluoxetine</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Paroxetine, 20-50 milligram per 1 day(s)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://trials.drugis.org/instances/1d5b7e1d-aa8e-46eb-8491-8d2510d7b314</t>
-  </si>
-  <si>
-    <t xml:space="preserve">baselineCharacteristic</t>
-  </si>
-  <si>
-    <t xml:space="preserve">continuous</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://trials.drugis.org/instances/e67b76fd-bfea-4d08-9409-7686702efeec</t>
-  </si>
-  <si>
-    <t xml:space="preserve">endpoint</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dichotomous</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fluoxetine + background metformin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fluoxetine, 20-6- milligram per 1 day(s) + metformin, 100 milligram per 1 day(s)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Overall population</t>
   </si>
   <si>
     <t xml:space="preserve">type</t>
@@ -434,8 +416,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -443,16 +433,12 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -476,124 +462,115 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AD6"/>
+  <dimension ref="A1:AA6"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Z4" activeCellId="0" sqref="Z4"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="P1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="W2" activeCellId="0" sqref="W2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="6" min="4" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="14.7142857142857"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.1683673469388"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="22" min="12" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="25" min="24" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="27" min="26" style="0" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="34.5561224489796"/>
-    <col collapsed="false" hidden="false" max="30" min="29" style="0" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="31" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="14.4438775510204"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="18.8979591836735"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="24" min="23" style="0" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="34.1530612244898"/>
+    <col collapsed="false" hidden="false" max="27" min="26" style="0" width="17.0102040816327"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="H1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="I1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="0" t="s">
+      <c r="J1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="K1" s="0" t="s">
+      <c r="K1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="L1" s="0" t="s">
+      <c r="L1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="M1" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="N1" s="0" t="s">
+      <c r="M1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="O1" s="0" t="s">
+      <c r="N1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="P1" s="0" t="s">
+      <c r="O1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="Q1" s="0" t="s">
+      <c r="P1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="R1" s="0" t="s">
+      <c r="Q1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="S1" s="0" t="s">
+      <c r="R1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="T1" s="0" t="s">
+      <c r="S1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="U1" s="0" t="s">
+      <c r="T1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="V1" s="0" t="s">
+      <c r="U1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="W1" s="0" t="s">
+      <c r="V1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="X1" s="0" t="s">
+      <c r="W1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="Y1" s="0" t="s">
+      <c r="X1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="Z1" s="0" t="s">
+      <c r="Y1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="AA1" s="0" t="s">
+      <c r="Z1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="AB1" s="0" t="s">
+      <c r="AA1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="AC1" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="AD1" s="0" t="s">
-        <v>3</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M2" s="0" t="str">
+        <f aca="false">Concepts!B6</f>
+        <v>HAMD bas</v>
+      </c>
       <c r="N2" s="0" t="str">
         <f aca="false">Concepts!B6</f>
         <v>HAMD bas</v>
@@ -631,12 +608,12 @@
         <v>HAMD bas</v>
       </c>
       <c r="W2" s="0" t="str">
-        <f aca="false">Concepts!B6</f>
-        <v>HAMD bas</v>
+        <f aca="false">Concepts!B7</f>
+        <v>HAM-D Responders</v>
       </c>
       <c r="X2" s="0" t="str">
-        <f aca="false">Concepts!B6</f>
-        <v>HAMD bas</v>
+        <f aca="false">Concepts!B7</f>
+        <v>HAM-D Responders</v>
       </c>
       <c r="Y2" s="0" t="str">
         <f aca="false">Concepts!B7</f>
@@ -650,18 +627,6 @@
         <f aca="false">Concepts!B7</f>
         <v>HAM-D Responders</v>
       </c>
-      <c r="AB2" s="0" t="str">
-        <f aca="false">Concepts!B7</f>
-        <v>HAM-D Responders</v>
-      </c>
-      <c r="AC2" s="0" t="str">
-        <f aca="false">Concepts!B7</f>
-        <v>HAM-D Responders</v>
-      </c>
-      <c r="AD2" s="0" t="str">
-        <f aca="false">Concepts!B7</f>
-        <v>HAM-D Responders</v>
-      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
@@ -719,10 +684,10 @@
         <v>20</v>
       </c>
       <c r="S3" s="0" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="T3" s="0" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="U3" s="0" t="s">
         <v>19</v>
@@ -731,308 +696,257 @@
         <v>20</v>
       </c>
       <c r="W3" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="X3" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y3" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="Z3" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="X3" s="0" t="s">
+      <c r="AA3" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="14.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="Y3" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="Z3" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="AA3" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="AB3" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="AC3" s="0" t="s">
+      <c r="B4" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="AD3" s="0" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="14.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="C4" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="D4" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="E4" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="F4" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E4" s="0" t="s">
+      <c r="G4" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F4" s="0" t="s">
+      <c r="I4" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="G4" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="H4" s="0" t="s">
+      <c r="J4" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="I4" s="0" t="s">
+      <c r="K4" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="M4" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="K4" s="0" t="s">
+      <c r="N4" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="M4" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="N4" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="O4" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="P4" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q4" s="3" t="str">
+      <c r="O4" s="1" t="str">
         <f aca="false">'Measurement moments'!B3</f>
         <v>Baseline</v>
       </c>
+      <c r="P4" s="4" t="n">
+        <v>3.8</v>
+      </c>
+      <c r="Q4" s="4" t="n">
+        <v>23.9</v>
+      </c>
       <c r="R4" s="4" t="n">
-        <v>3.8</v>
-      </c>
-      <c r="S4" s="4" t="n">
-        <v>23.9</v>
-      </c>
-      <c r="T4" s="4" t="n">
         <v>54</v>
       </c>
-      <c r="U4" s="0" t="str">
+      <c r="S4" s="1" t="str">
         <f aca="false">'Measurement moments'!B2</f>
         <v>P0D BEFORE_EPOCH_END Main phase</v>
       </c>
+      <c r="T4" s="4" t="n">
+        <v>3.8</v>
+      </c>
+      <c r="U4" s="4" t="n">
+        <v>23.9</v>
+      </c>
       <c r="V4" s="4" t="n">
-        <v>3.8</v>
-      </c>
-      <c r="W4" s="4" t="n">
-        <v>23.9</v>
-      </c>
-      <c r="X4" s="4" t="n">
         <v>54</v>
       </c>
-      <c r="Y4" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="Z4" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="AA4" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="AB4" s="0" t="str">
+      <c r="W4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="X4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Y4" s="1" t="str">
         <f aca="false">'Measurement moments'!B2</f>
         <v>P0D BEFORE_EPOCH_END Main phase</v>
       </c>
-      <c r="AC4" s="0" t="n">
+      <c r="Z4" s="0" t="n">
         <v>31</v>
       </c>
-      <c r="AD4" s="0" t="n">
+      <c r="AA4" s="0" t="n">
         <v>54</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="D5" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="E5" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="F5" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="G5" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="H5" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="I5" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="J5" s="1" t="s">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="M5" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="K5" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="M5" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="N5" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="O5" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="P5" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q5" s="3" t="str">
+      <c r="N5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O5" s="1" t="str">
         <f aca="false">'Measurement moments'!B3</f>
         <v>Baseline</v>
       </c>
+      <c r="P5" s="4" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="Q5" s="4" t="n">
+        <v>22.9</v>
+      </c>
       <c r="R5" s="4" t="n">
-        <v>3.7</v>
-      </c>
-      <c r="S5" s="4" t="n">
-        <v>22.9</v>
-      </c>
-      <c r="T5" s="4" t="n">
         <v>52</v>
       </c>
-      <c r="U5" s="3" t="str">
+      <c r="S5" s="1" t="str">
         <f aca="false">'Measurement moments'!B2</f>
         <v>P0D BEFORE_EPOCH_END Main phase</v>
       </c>
+      <c r="T5" s="4" t="n">
+        <v>2.8</v>
+      </c>
+      <c r="U5" s="4" t="n">
+        <v>21.9</v>
+      </c>
       <c r="V5" s="4" t="n">
-        <v>2.8</v>
-      </c>
-      <c r="W5" s="4" t="n">
-        <v>21.9</v>
-      </c>
-      <c r="X5" s="4" t="n">
         <v>52</v>
       </c>
-      <c r="Y5" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="Z5" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="AA5" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="AB5" s="3" t="str">
+      <c r="W5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="X5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Y5" s="1" t="str">
         <f aca="false">'Measurement moments'!B2</f>
         <v>P0D BEFORE_EPOCH_END Main phase</v>
       </c>
-      <c r="AC5" s="0" t="n">
+      <c r="Z5" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="AD5" s="0" t="n">
+      <c r="AA5" s="0" t="n">
         <v>52</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="D6" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="E6" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="F6" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="G6" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="H6" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="I6" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="J6" s="1" t="s">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="M6" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="K6" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="N6" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="O6" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="P6" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q6" s="3" t="str">
+      <c r="N6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O6" s="1" t="str">
         <f aca="false">'Measurement moments'!B3</f>
         <v>Baseline</v>
       </c>
+      <c r="P6" s="4" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="Q6" s="4" t="n">
+        <v>23.5</v>
+      </c>
       <c r="R6" s="4" t="n">
-        <v>3.5</v>
-      </c>
-      <c r="S6" s="4" t="n">
-        <v>23.5</v>
-      </c>
-      <c r="T6" s="4" t="n">
         <v>106</v>
       </c>
-      <c r="U6" s="3" t="str">
+      <c r="S6" s="1" t="str">
         <f aca="false">'Measurement moments'!B2</f>
         <v>P0D BEFORE_EPOCH_END Main phase</v>
       </c>
+      <c r="T6" s="4" t="n">
+        <v>2.8</v>
+      </c>
+      <c r="U6" s="4" t="n">
+        <v>21.9</v>
+      </c>
       <c r="V6" s="4" t="n">
-        <v>2.8</v>
-      </c>
-      <c r="W6" s="4" t="n">
-        <v>21.9</v>
-      </c>
-      <c r="X6" s="4" t="n">
         <v>52</v>
       </c>
-      <c r="Y6" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="Z6" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="AA6" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="AB6" s="3" t="str">
+      <c r="W6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="X6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Y6" s="1" t="str">
         <f aca="false">'Measurement moments'!B2</f>
         <v>P0D BEFORE_EPOCH_END Main phase</v>
       </c>
-      <c r="AC6" s="0" t="n">
+      <c r="Z6" s="0" t="n">
         <v>63</v>
       </c>
-      <c r="AD6" s="0" t="n">
+      <c r="AA6" s="0" t="n">
         <v>106</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="22">
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="K1:L1"/>
+    <mergeCell ref="M1:AA1"/>
+    <mergeCell ref="M2:V2"/>
+    <mergeCell ref="W2:AA2"/>
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="B4:B6"/>
+    <mergeCell ref="C4:C6"/>
+    <mergeCell ref="D4:D6"/>
+    <mergeCell ref="E4:E6"/>
+    <mergeCell ref="F4:F6"/>
+    <mergeCell ref="G4:G6"/>
+    <mergeCell ref="H4:H6"/>
+    <mergeCell ref="I4:I6"/>
+    <mergeCell ref="M4:M6"/>
+    <mergeCell ref="N4:N6"/>
+    <mergeCell ref="O4:O6"/>
+    <mergeCell ref="S4:S6"/>
+    <mergeCell ref="W4:W6"/>
+    <mergeCell ref="X4:X6"/>
+    <mergeCell ref="Y4:Y6"/>
+  </mergeCells>
   <hyperlinks>
-    <hyperlink ref="N4" r:id="rId1" display="http://trials.drugis.org/instances/1d5b7e1d-aa8e-46eb-8491-8d2510d7b314"/>
-    <hyperlink ref="N5" r:id="rId2" display="http://trials.drugis.org/instances/1d5b7e1d-aa8e-46eb-8491-8d2510d7b314"/>
-    <hyperlink ref="N6" r:id="rId3" display="http://trials.drugis.org/instances/1d5b7e1d-aa8e-46eb-8491-8d2510d7b314"/>
+    <hyperlink ref="B4" r:id="rId1" location="/users/4/datasets/215004da-4ef3-4979-afb1-24be42bb0ecf/versions/62411d0c-d327-431d-854a-3715b895413a/studies/5e759104-6992-429c-91a4-ff9779c1f14a" display="https://addis-test.drugis.org/#/users/4/datasets/215004da-4ef3-4979-afb1-24be42bb0ecf/versions/62411d0c-d327-431d-854a-3715b895413a/studies/5e759104-6992-429c-91a4-ff9779c1f14a"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -1051,114 +965,111 @@
   </sheetPr>
   <dimension ref="A1:P6"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K7" activeCellId="0" sqref="K7"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K6" activeCellId="0" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>16</v>
+        <v>38</v>
       </c>
       <c r="B1" s="0" t="s">
         <v>6</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="D1" s="0" t="s">
         <v>14</v>
       </c>
       <c r="E1" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="J1" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="K1" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="L1" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="M1" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="N1" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="O1" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="P1" s="0" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="B2" s="0" t="s">
         <v>47</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="C2" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="B3" s="0" t="s">
         <v>49</v>
       </c>
-      <c r="J1" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="K1" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="L1" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="M1" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="N1" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="O1" s="0" t="s">
+      <c r="C3" s="0" t="s">
         <v>49</v>
-      </c>
-      <c r="P1" s="0" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="E5" s="0" t="str">
         <f aca="false">Concepts!B2</f>
         <v>Paroxetine</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="G5" s="0" t="n">
         <v>20</v>
@@ -1167,28 +1078,28 @@
         <v>50</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="J5" s="0" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="E6" s="0" t="str">
         <f aca="false">Concepts!B3</f>
         <v>Fluoxetine</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="G6" s="0" t="n">
         <v>20</v>
@@ -1197,26 +1108,26 @@
         <v>50</v>
       </c>
       <c r="I6" s="0" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="J6" s="0" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="K6" s="0" t="str">
         <f aca="false">Concepts!B4</f>
         <v>Metformin</v>
       </c>
       <c r="L6" s="0" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="M6" s="0" t="n">
         <v>100</v>
       </c>
       <c r="O6" s="0" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="P6" s="0" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -1246,83 +1157,80 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>16</v>
+        <v>38</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="C1" s="0" t="s">
         <v>14</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="E2" s="5" t="n">
+        <v>63</v>
+      </c>
+      <c r="E2" s="6" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="E3" s="5" t="n">
+        <v>66</v>
+      </c>
+      <c r="E3" s="6" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="E4" s="5" t="n">
+        <v>63</v>
+      </c>
+      <c r="E4" s="6" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>75</v>
-      </c>
-      <c r="E5" s="5" t="n">
+        <v>70</v>
+      </c>
+      <c r="E5" s="6" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -1350,13 +1258,10 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="B1" s="0" t="str">
         <f aca="false">Epochs!B2</f>
@@ -1370,7 +1275,7 @@
         <f aca="false">Epochs!B4</f>
         <v>Randomization</v>
       </c>
-      <c r="E1" s="5" t="str">
+      <c r="E1" s="6" t="str">
         <f aca="false">Epochs!B5</f>
         <v>Main phase</v>
       </c>
@@ -1442,61 +1347,58 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>16</v>
+        <v>38</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="C2" s="0" t="str">
         <f aca="false">Epochs!B5</f>
         <v>Main phase</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C3" s="0" t="str">
         <f aca="false">Epochs!B5</f>
         <v>Main phase</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -1523,83 +1425,81 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.63775510204082"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>16</v>
+        <v>38</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>92</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>33</v>
+        <v>87</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>31</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>94</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>95</v>
+        <v>89</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>90</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="E5" s="0" t="n">
         <v>0.001</v>
@@ -1607,30 +1507,30 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>